<commit_message>
Fix sheet name to be "urls"
</commit_message>
<xml_diff>
--- a/urls_test_for_fixing_empty_llm_calls.xlsx
+++ b/urls_test_for_fixing_empty_llm_calls.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMulvaneyKemp\Documents\repos\AI_parser_pipeline_github\aiparserpipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3C2E959-B2F4-47AD-BC4D-73B2ECA13904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440B75BF-C328-46C5-9889-D826DA8D432F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{205982ED-6EB9-47A4-8552-D5048CBCBC47}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="urls" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>

</xml_diff>

<commit_message>
new test file with dummy urls that don't exist
</commit_message>
<xml_diff>
--- a/urls_test_for_fixing_empty_llm_calls.xlsx
+++ b/urls_test_for_fixing_empty_llm_calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMulvaneyKemp\Documents\repos\AI_parser_pipeline_github\aiparserpipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4C83CA-3B0F-4D96-9853-34A68DA6D368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCF03D2-7334-4B0B-A0BB-E2213CDA96CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{205982ED-6EB9-47A4-8552-D5048CBCBC47}"/>
   </bookViews>
@@ -36,16 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Washington County Solar</t>
-  </si>
-  <si>
-    <t>Baldwin Solar BESS</t>
-  </si>
-  <si>
-    <t>Gemini Solar</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>https://texaselectricnews.com/archives-2020/</t>
   </si>
@@ -53,9 +44,6 @@
     <t>Arroyo Solar Energy Storage Hybrid</t>
   </si>
   <si>
-    <t>https://www.quinbrook.com/news-insights/historic-gemini-solar-energy-storage-project-reaches-commercial-operations-in-nevada/</t>
-  </si>
-  <si>
     <t>https://www.dnb.com/business-directory/company-profiles.aeug_union_solar_llc.4319009bfa1d1f19f7cbdd9aeccbe0d4.html</t>
   </si>
   <si>
@@ -71,50 +59,52 @@
     <t>https://portal.pennaeps.com/app/publiccontroller/view_QFs/1/pv_total_inverter_capacity/desc/</t>
   </si>
   <si>
-    <t>https://www-entergynewsroom-532530194.us-east-1.elb.amazonaws.com/article/west-memphis-project-companys-largest-solar-project-so-far/</t>
-  </si>
-  <si>
-    <t>West Memphis Solar Station</t>
-  </si>
-  <si>
     <t>https://www.ecowatch.com/solar/best-solar-powered-ac</t>
   </si>
   <si>
-    <t>https://www.41nbc.com/washington-county/</t>
-  </si>
-  <si>
-    <t>https://www.kmdpower.com/news/ac-vs-dc-coupled-bess/</t>
-  </si>
-  <si>
-    <t>https://www.cnet.com/home/solar/which-states-have-community-solar-find-out-here/</t>
-  </si>
-  <si>
-    <t>https://www.dnb.com/business-directory/company-profiles.sorrentino_development_corp.d0403695ea6cff6c828231ec0315fab7.html</t>
-  </si>
-  <si>
-    <t>NY Sorrell Hill II CSG</t>
-  </si>
-  <si>
-    <t>https://documents.dps.ny.gov/public/Common/ViewDoc.aspx?DocRefId=%7B650846FC-48AC-45E5-9672-9300CABC2198%7D</t>
-  </si>
-  <si>
-    <t>https://electrek.co/2025/01/08/florida-solar-farm-is-supplying-clean-energy-to-12-cities/</t>
-  </si>
-  <si>
-    <t>English Creek Solar</t>
-  </si>
-  <si>
-    <t>https://www.tampabay.com/news/business/2025/05/29/congress-could-kill-rooftop-solar-tax-credits-used-by-florida-homeowners/</t>
+    <t>https://ww.jmk.org/</t>
+  </si>
+  <si>
+    <t>https://ww.jmkk.org/</t>
+  </si>
+  <si>
+    <t>https://www.vasolarllc.com/project/nokesville-solar/</t>
+  </si>
+  <si>
+    <t>Dummy Project</t>
+  </si>
+  <si>
+    <t>https://www.dentoncounty.gov/AgendaCenter/ViewFile/Agenda/_12162020-484</t>
+  </si>
+  <si>
+    <t>https://www.businesswire.com/news/home/20220208005079/en/Silicon-Ranch-Selects-Black-Veatch-to-Build-125-Megawatt-Solar-Farm-in-Georgia</t>
+  </si>
+  <si>
+    <t>https://www.powerfinancerisk.com/article/28pgamro23ti2n3wgre2o/real-estate-developer-seeks-buyer-for-sc-solar-project</t>
+  </si>
+  <si>
+    <t>https://www.dbusiness.com/daily-news/three-major-solar-power-projects-coming-to-michigan/</t>
+  </si>
+  <si>
+    <t>https://www.marathoncapital.com/transactions/spower</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -137,13 +127,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,101 +469,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D9D5B6-20D3-4BE1-B6C1-2DE4DAF154F5}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="H3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{1544D526-1E3E-4A3D-B2C6-6AA6679BA0E7}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added pipeline log entry when scraping not successful; adjusted catch location in get_api_response for short article text
</commit_message>
<xml_diff>
--- a/urls_test_for_fixing_empty_llm_calls.xlsx
+++ b/urls_test_for_fixing_empty_llm_calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMulvaneyKemp\Documents\repos\AI_parser_pipeline_github\aiparserpipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCF03D2-7334-4B0B-A0BB-E2213CDA96CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9441CAF0-B347-4DCB-8427-1A224FB400D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{205982ED-6EB9-47A4-8552-D5048CBCBC47}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>https://texaselectricnews.com/archives-2020/</t>
   </si>
@@ -77,16 +77,7 @@
     <t>https://www.dentoncounty.gov/AgendaCenter/ViewFile/Agenda/_12162020-484</t>
   </si>
   <si>
-    <t>https://www.businesswire.com/news/home/20220208005079/en/Silicon-Ranch-Selects-Black-Veatch-to-Build-125-Megawatt-Solar-Farm-in-Georgia</t>
-  </si>
-  <si>
-    <t>https://www.powerfinancerisk.com/article/28pgamro23ti2n3wgre2o/real-estate-developer-seeks-buyer-for-sc-solar-project</t>
-  </si>
-  <si>
     <t>https://www.dbusiness.com/daily-news/three-major-solar-power-projects-coming-to-michigan/</t>
-  </si>
-  <si>
-    <t>https://www.marathoncapital.com/transactions/spower</t>
   </si>
 </sst>
 </file>
@@ -469,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D9D5B6-20D3-4BE1-B6C1-2DE4DAF154F5}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -537,21 +528,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" xr:uid="{1544D526-1E3E-4A3D-B2C6-6AA6679BA0E7}"/>

</xml_diff>

<commit_message>
running main now requires submitting the excel path as an argument. Will enable batch run files to specify url list.
</commit_message>
<xml_diff>
--- a/urls_test_for_fixing_empty_llm_calls.xlsx
+++ b/urls_test_for_fixing_empty_llm_calls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JMulvaneyKemp\Documents\repos\AI_parser_pipeline_github\aiparserpipeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9441CAF0-B347-4DCB-8427-1A224FB400D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843AF5ED-B963-46F9-8D6E-BD430BDA8CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{205982ED-6EB9-47A4-8552-D5048CBCBC47}"/>
   </bookViews>
@@ -36,24 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>https://texaselectricnews.com/archives-2020/</t>
-  </si>
-  <si>
-    <t>Arroyo Solar Energy Storage Hybrid</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>https://www.dnb.com/business-directory/company-profiles.aeug_union_solar_llc.4319009bfa1d1f19f7cbdd9aeccbe0d4.html</t>
   </si>
   <si>
     <t>AEUG Union Solar, LLC</t>
-  </si>
-  <si>
-    <t>https://www.newsweek.com/billion-dollar-solar-farm-planned-wyoming-1899773</t>
-  </si>
-  <si>
-    <t>South Cheyenne Solar</t>
   </si>
   <si>
     <t>https://portal.pennaeps.com/app/publiccontroller/view_QFs/1/pv_total_inverter_capacity/desc/</t>
@@ -460,72 +448,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9D9D5B6-20D3-4BE1-B6C1-2DE4DAF154F5}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>